<commit_message>
:recycle: Dot to comma prompt improvement
</commit_message>
<xml_diff>
--- a/assets/docs_output/Execução - 18_12_2024 - Execution_data Template.xlsx
+++ b/assets/docs_output/Execução - 18_12_2024 - Execution_data Template.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -655,7 +655,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -694,7 +694,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -772,7 +772,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -811,7 +811,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -850,7 +850,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -928,7 +928,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -967,7 +967,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1084,7 +1084,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1396,7 +1396,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1630,7 +1630,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1825,7 +1825,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2020,7 +2020,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2059,7 +2059,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2137,7 +2137,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -2215,7 +2215,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -2254,7 +2254,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2332,7 +2332,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2371,7 +2371,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2449,7 +2449,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2488,7 +2488,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2527,7 +2527,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2644,7 +2644,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2683,7 +2683,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2722,7 +2722,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2761,7 +2761,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2800,7 +2800,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2839,7 +2839,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2878,7 +2878,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2917,7 +2917,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2956,7 +2956,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2995,7 +2995,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3073,7 +3073,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -3112,7 +3112,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -3151,7 +3151,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -3190,7 +3190,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3229,7 +3229,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3268,7 +3268,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -3385,7 +3385,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -3424,7 +3424,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -3463,7 +3463,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -3502,7 +3502,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -3580,7 +3580,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -3619,7 +3619,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3658,7 +3658,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -3697,7 +3697,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -3736,7 +3736,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -3775,7 +3775,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3814,7 +3814,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -3853,7 +3853,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -3892,7 +3892,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -3931,7 +3931,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -3970,7 +3970,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -4009,7 +4009,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -4048,7 +4048,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
@@ -4087,7 +4087,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -4126,7 +4126,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -4165,7 +4165,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -4204,7 +4204,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -4243,7 +4243,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
@@ -4282,7 +4282,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -4360,7 +4360,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
@@ -4399,7 +4399,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
@@ -4438,7 +4438,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -4477,7 +4477,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -4516,7 +4516,7 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -4555,7 +4555,7 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -4594,7 +4594,7 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -4633,7 +4633,7 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -4672,7 +4672,7 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -4711,7 +4711,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
@@ -4750,7 +4750,7 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
@@ -4828,7 +4828,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -4867,7 +4867,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -4906,7 +4906,7 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -4945,7 +4945,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -4984,7 +4984,7 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
@@ -5023,7 +5023,7 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
@@ -5062,7 +5062,7 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -5140,7 +5140,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
@@ -5179,7 +5179,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
@@ -5218,7 +5218,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
@@ -5257,7 +5257,7 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
@@ -5296,7 +5296,7 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -5335,7 +5335,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
@@ -5374,7 +5374,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
@@ -5413,7 +5413,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -5452,7 +5452,7 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -5491,7 +5491,7 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -5530,7 +5530,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -5569,7 +5569,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -5608,7 +5608,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -5647,7 +5647,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -5686,7 +5686,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
@@ -5725,7 +5725,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
@@ -5764,7 +5764,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -5803,7 +5803,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
@@ -5842,7 +5842,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
@@ -5920,7 +5920,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
@@ -5959,7 +5959,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -6037,7 +6037,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -6076,7 +6076,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
@@ -6115,7 +6115,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
@@ -6154,7 +6154,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -6193,7 +6193,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -6232,7 +6232,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -6271,7 +6271,7 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -6310,7 +6310,7 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -6349,7 +6349,7 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -6388,7 +6388,7 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
@@ -6427,7 +6427,7 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
@@ -6466,7 +6466,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
@@ -6505,7 +6505,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
@@ -6544,7 +6544,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -6583,7 +6583,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -6622,7 +6622,7 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
@@ -6700,7 +6700,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -6739,7 +6739,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
@@ -6778,7 +6778,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -6817,7 +6817,7 @@
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -6856,7 +6856,7 @@
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -6895,7 +6895,7 @@
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -6934,7 +6934,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F167" t="inlineStr">
@@ -6973,7 +6973,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -7012,7 +7012,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -7051,7 +7051,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -7090,7 +7090,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
@@ -7129,7 +7129,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F172" t="inlineStr">
@@ -7168,7 +7168,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F173" t="inlineStr">
@@ -7207,7 +7207,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -7246,7 +7246,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -7285,7 +7285,7 @@
       </c>
       <c r="E176" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F176" t="inlineStr">
@@ -7324,7 +7324,7 @@
       </c>
       <c r="E177" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F177" t="inlineStr">
@@ -7363,7 +7363,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
@@ -7402,7 +7402,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -7441,7 +7441,7 @@
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
@@ -7480,7 +7480,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -7519,7 +7519,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
@@ -7558,7 +7558,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F183" t="inlineStr">
@@ -7597,7 +7597,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
@@ -7636,7 +7636,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
@@ -7675,7 +7675,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -7714,7 +7714,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -7753,7 +7753,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -7792,7 +7792,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -7831,7 +7831,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -7870,7 +7870,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -7909,7 +7909,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
@@ -7948,7 +7948,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
@@ -7987,7 +7987,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
@@ -8026,7 +8026,7 @@
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
@@ -8065,7 +8065,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
@@ -8104,7 +8104,7 @@
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -8143,7 +8143,7 @@
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -8182,7 +8182,7 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -8221,7 +8221,7 @@
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
@@ -8260,7 +8260,7 @@
       </c>
       <c r="E201" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F201" t="inlineStr">
@@ -8299,7 +8299,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -8338,7 +8338,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -8377,7 +8377,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -8416,7 +8416,7 @@
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -8455,7 +8455,7 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -8494,7 +8494,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -8533,7 +8533,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -8572,7 +8572,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -8611,7 +8611,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -8650,7 +8650,7 @@
       </c>
       <c r="E211" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -8689,7 +8689,7 @@
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -8728,7 +8728,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -8767,7 +8767,7 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -8806,7 +8806,7 @@
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -8845,7 +8845,7 @@
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -8884,7 +8884,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -8923,7 +8923,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -8962,7 +8962,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -9040,7 +9040,7 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -9079,7 +9079,7 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -9118,7 +9118,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -9157,7 +9157,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -9196,7 +9196,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -9235,7 +9235,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -9274,7 +9274,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -9313,7 +9313,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -9352,7 +9352,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -9391,7 +9391,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -9430,7 +9430,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -9469,7 +9469,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -9508,7 +9508,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -9547,7 +9547,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -9586,7 +9586,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -9625,7 +9625,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -9664,7 +9664,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -9703,7 +9703,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -9742,7 +9742,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -9781,7 +9781,7 @@
       </c>
       <c r="E240" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -9820,7 +9820,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -9859,7 +9859,7 @@
       </c>
       <c r="E242" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -9898,7 +9898,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -9937,7 +9937,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -9976,7 +9976,7 @@
       </c>
       <c r="E245" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -10015,7 +10015,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -10054,7 +10054,7 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -10093,7 +10093,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -10132,7 +10132,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -10171,7 +10171,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -10210,7 +10210,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -10249,7 +10249,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -10288,7 +10288,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -10327,7 +10327,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -10366,7 +10366,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
@@ -10405,7 +10405,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -10444,7 +10444,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F257" t="inlineStr">
@@ -10483,7 +10483,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -10522,7 +10522,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -10561,7 +10561,7 @@
       </c>
       <c r="E260" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
@@ -10600,7 +10600,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F261" t="inlineStr">
@@ -10639,7 +10639,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -10678,7 +10678,7 @@
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -10717,7 +10717,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
@@ -10756,7 +10756,7 @@
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
@@ -10795,7 +10795,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
@@ -10834,7 +10834,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F267" t="inlineStr">
@@ -10873,7 +10873,7 @@
       </c>
       <c r="E268" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F268" t="inlineStr">
@@ -10912,7 +10912,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -10951,7 +10951,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -10990,7 +10990,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -11029,7 +11029,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
@@ -11068,7 +11068,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F273" t="inlineStr">
@@ -11107,7 +11107,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -11146,7 +11146,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
@@ -11185,7 +11185,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F276" t="inlineStr">
@@ -11224,7 +11224,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -11263,7 +11263,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -11302,7 +11302,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -11341,7 +11341,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -11380,7 +11380,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F281" t="inlineStr">
@@ -11419,7 +11419,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -11458,7 +11458,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F283" t="inlineStr">
@@ -11497,7 +11497,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -11536,7 +11536,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -11575,7 +11575,7 @@
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F286" t="inlineStr">
@@ -11614,7 +11614,7 @@
       </c>
       <c r="E287" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F287" t="inlineStr">
@@ -11653,7 +11653,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -11692,7 +11692,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -11731,7 +11731,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
@@ -11770,7 +11770,7 @@
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
@@ -11809,7 +11809,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -11848,7 +11848,7 @@
       </c>
       <c r="E293" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F293" t="inlineStr">
@@ -11887,7 +11887,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
@@ -11926,7 +11926,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
@@ -11965,7 +11965,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F296" t="inlineStr">
@@ -12004,7 +12004,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
@@ -12043,7 +12043,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F298" t="inlineStr">
@@ -12082,7 +12082,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -12121,7 +12121,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
@@ -12160,7 +12160,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
@@ -12199,7 +12199,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -12238,7 +12238,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
@@ -12277,7 +12277,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F304" t="inlineStr">
@@ -12316,7 +12316,7 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
@@ -12355,7 +12355,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F306" t="inlineStr">
@@ -12394,7 +12394,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -12433,7 +12433,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -12472,7 +12472,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -12511,7 +12511,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
@@ -12550,7 +12550,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F311" t="inlineStr">
@@ -12589,7 +12589,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -12628,7 +12628,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
@@ -12667,7 +12667,7 @@
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -12706,7 +12706,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
@@ -12745,7 +12745,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -12784,7 +12784,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
@@ -12823,7 +12823,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -12862,7 +12862,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F319" t="inlineStr">
@@ -12901,7 +12901,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -12940,7 +12940,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -12979,7 +12979,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F322" t="inlineStr">
@@ -13018,7 +13018,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
@@ -13057,7 +13057,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F324" t="inlineStr">
@@ -13096,7 +13096,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F325" t="inlineStr">
@@ -13135,7 +13135,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -13174,7 +13174,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
@@ -13213,7 +13213,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F328" t="inlineStr">
@@ -13252,7 +13252,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
@@ -13291,7 +13291,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F330" t="inlineStr">
@@ -13330,7 +13330,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -13369,7 +13369,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
@@ -13408,7 +13408,7 @@
       </c>
       <c r="E333" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
@@ -13447,7 +13447,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -13486,7 +13486,7 @@
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
@@ -13525,7 +13525,7 @@
       </c>
       <c r="E336" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F336" t="inlineStr">
@@ -13564,7 +13564,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
@@ -13603,7 +13603,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -13642,7 +13642,7 @@
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -13681,7 +13681,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
@@ -13720,7 +13720,7 @@
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
@@ -13759,7 +13759,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
@@ -13798,7 +13798,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
@@ -13837,7 +13837,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
@@ -13876,7 +13876,7 @@
       </c>
       <c r="E345" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F345" t="inlineStr">
@@ -13915,7 +13915,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -13954,7 +13954,7 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F347" t="inlineStr">
@@ -13993,7 +13993,7 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
@@ -14032,7 +14032,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
@@ -14071,7 +14071,7 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
@@ -14110,7 +14110,7 @@
       </c>
       <c r="E351" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F351" t="inlineStr">
@@ -14149,7 +14149,7 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F352" t="inlineStr">
@@ -14188,7 +14188,7 @@
       </c>
       <c r="E353" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
@@ -14227,7 +14227,7 @@
       </c>
       <c r="E354" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F354" t="inlineStr">
@@ -14266,7 +14266,7 @@
       </c>
       <c r="E355" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F355" t="inlineStr">
@@ -14305,7 +14305,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F356" t="inlineStr">
@@ -14344,7 +14344,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F357" t="inlineStr">
@@ -14383,7 +14383,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F358" t="inlineStr">
@@ -14422,7 +14422,7 @@
       </c>
       <c r="E359" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F359" t="inlineStr">
@@ -14461,7 +14461,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F360" t="inlineStr">
@@ -14500,7 +14500,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F361" t="inlineStr">
@@ -14539,7 +14539,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F362" t="inlineStr">
@@ -14578,7 +14578,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F363" t="inlineStr">
@@ -14617,7 +14617,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F364" t="inlineStr">
@@ -14656,7 +14656,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F365" t="inlineStr">
@@ -14695,7 +14695,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F366" t="inlineStr">
@@ -14734,7 +14734,7 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F367" t="inlineStr">
@@ -14773,7 +14773,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F368" t="inlineStr">
@@ -14812,7 +14812,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F369" t="inlineStr">
@@ -14851,7 +14851,7 @@
       </c>
       <c r="E370" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F370" t="inlineStr">
@@ -14890,7 +14890,7 @@
       </c>
       <c r="E371" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F371" t="inlineStr">
@@ -14929,7 +14929,7 @@
       </c>
       <c r="E372" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F372" t="inlineStr">
@@ -14968,7 +14968,7 @@
       </c>
       <c r="E373" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
@@ -15007,7 +15007,7 @@
       </c>
       <c r="E374" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F374" t="inlineStr">
@@ -15046,7 +15046,7 @@
       </c>
       <c r="E375" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F375" t="inlineStr">
@@ -15085,7 +15085,7 @@
       </c>
       <c r="E376" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F376" t="inlineStr">
@@ -15124,7 +15124,7 @@
       </c>
       <c r="E377" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F377" t="inlineStr">
@@ -15163,7 +15163,7 @@
       </c>
       <c r="E378" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F378" t="inlineStr">
@@ -15202,7 +15202,7 @@
       </c>
       <c r="E379" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F379" t="inlineStr">
@@ -15241,7 +15241,7 @@
       </c>
       <c r="E380" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F380" t="inlineStr">
@@ -15280,7 +15280,7 @@
       </c>
       <c r="E381" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F381" t="inlineStr">
@@ -15319,7 +15319,7 @@
       </c>
       <c r="E382" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F382" t="inlineStr">
@@ -15358,7 +15358,7 @@
       </c>
       <c r="E383" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F383" t="inlineStr">
@@ -15397,7 +15397,7 @@
       </c>
       <c r="E384" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F384" t="inlineStr">
@@ -15436,7 +15436,7 @@
       </c>
       <c r="E385" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F385" t="inlineStr">
@@ -15475,7 +15475,7 @@
       </c>
       <c r="E386" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F386" t="inlineStr">
@@ -15514,7 +15514,7 @@
       </c>
       <c r="E387" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F387" t="inlineStr">
@@ -15553,7 +15553,7 @@
       </c>
       <c r="E388" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F388" t="inlineStr">
@@ -15592,7 +15592,7 @@
       </c>
       <c r="E389" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F389" t="inlineStr">
@@ -15631,7 +15631,7 @@
       </c>
       <c r="E390" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F390" t="inlineStr">
@@ -15670,7 +15670,7 @@
       </c>
       <c r="E391" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F391" t="inlineStr">
@@ -15709,7 +15709,7 @@
       </c>
       <c r="E392" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F392" t="inlineStr">
@@ -15748,7 +15748,7 @@
       </c>
       <c r="E393" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F393" t="inlineStr">
@@ -15787,7 +15787,7 @@
       </c>
       <c r="E394" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F394" t="inlineStr">
@@ -15826,7 +15826,7 @@
       </c>
       <c r="E395" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F395" t="inlineStr">
@@ -15865,7 +15865,7 @@
       </c>
       <c r="E396" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F396" t="inlineStr">
@@ -15904,7 +15904,7 @@
       </c>
       <c r="E397" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F397" t="inlineStr">
@@ -15943,7 +15943,7 @@
       </c>
       <c r="E398" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F398" t="inlineStr">
@@ -15982,7 +15982,7 @@
       </c>
       <c r="E399" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F399" t="inlineStr">
@@ -16021,7 +16021,7 @@
       </c>
       <c r="E400" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F400" t="inlineStr">
@@ -16060,7 +16060,7 @@
       </c>
       <c r="E401" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F401" t="inlineStr">
@@ -16099,7 +16099,7 @@
       </c>
       <c r="E402" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F402" t="inlineStr">
@@ -16138,7 +16138,7 @@
       </c>
       <c r="E403" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F403" t="inlineStr">
@@ -16177,7 +16177,7 @@
       </c>
       <c r="E404" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F404" t="inlineStr">
@@ -16216,7 +16216,7 @@
       </c>
       <c r="E405" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F405" t="inlineStr">
@@ -16255,7 +16255,7 @@
       </c>
       <c r="E406" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F406" t="inlineStr">
@@ -16294,7 +16294,7 @@
       </c>
       <c r="E407" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F407" t="inlineStr">
@@ -16333,7 +16333,7 @@
       </c>
       <c r="E408" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F408" t="inlineStr">
@@ -16372,7 +16372,7 @@
       </c>
       <c r="E409" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F409" t="inlineStr">
@@ -16411,7 +16411,7 @@
       </c>
       <c r="E410" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F410" t="inlineStr">
@@ -16450,7 +16450,7 @@
       </c>
       <c r="E411" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F411" t="inlineStr">
@@ -16489,7 +16489,7 @@
       </c>
       <c r="E412" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F412" t="inlineStr">
@@ -16528,7 +16528,7 @@
       </c>
       <c r="E413" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F413" t="inlineStr">
@@ -16567,7 +16567,7 @@
       </c>
       <c r="E414" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F414" t="inlineStr">
@@ -16606,7 +16606,7 @@
       </c>
       <c r="E415" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F415" t="inlineStr">
@@ -16645,7 +16645,7 @@
       </c>
       <c r="E416" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F416" t="inlineStr">
@@ -16684,7 +16684,7 @@
       </c>
       <c r="E417" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F417" t="inlineStr">
@@ -16723,7 +16723,7 @@
       </c>
       <c r="E418" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F418" t="inlineStr">
@@ -16762,7 +16762,7 @@
       </c>
       <c r="E419" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F419" t="inlineStr">
@@ -16801,7 +16801,7 @@
       </c>
       <c r="E420" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F420" t="inlineStr">
@@ -16840,7 +16840,7 @@
       </c>
       <c r="E421" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F421" t="inlineStr">
@@ -16879,7 +16879,7 @@
       </c>
       <c r="E422" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F422" t="inlineStr">
@@ -16918,7 +16918,7 @@
       </c>
       <c r="E423" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F423" t="inlineStr">
@@ -16957,7 +16957,7 @@
       </c>
       <c r="E424" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F424" t="inlineStr">
@@ -16996,7 +16996,7 @@
       </c>
       <c r="E425" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F425" t="inlineStr">
@@ -17035,7 +17035,7 @@
       </c>
       <c r="E426" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F426" t="inlineStr">
@@ -17074,7 +17074,7 @@
       </c>
       <c r="E427" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F427" t="inlineStr">
@@ -17113,7 +17113,7 @@
       </c>
       <c r="E428" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F428" t="inlineStr">
@@ -17152,7 +17152,7 @@
       </c>
       <c r="E429" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F429" t="inlineStr">
@@ -17191,7 +17191,7 @@
       </c>
       <c r="E430" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F430" t="inlineStr">
@@ -17230,7 +17230,7 @@
       </c>
       <c r="E431" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F431" t="inlineStr">
@@ -17269,7 +17269,7 @@
       </c>
       <c r="E432" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F432" t="inlineStr">
@@ -17308,7 +17308,7 @@
       </c>
       <c r="E433" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F433" t="inlineStr">
@@ -17347,7 +17347,7 @@
       </c>
       <c r="E434" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F434" t="inlineStr">
@@ -17386,7 +17386,7 @@
       </c>
       <c r="E435" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F435" t="inlineStr">
@@ -17425,7 +17425,7 @@
       </c>
       <c r="E436" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F436" t="inlineStr">
@@ -17464,7 +17464,7 @@
       </c>
       <c r="E437" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F437" t="inlineStr">
@@ -17503,7 +17503,7 @@
       </c>
       <c r="E438" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F438" t="inlineStr">
@@ -17542,7 +17542,7 @@
       </c>
       <c r="E439" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F439" t="inlineStr">
@@ -17581,7 +17581,7 @@
       </c>
       <c r="E440" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F440" t="inlineStr">
@@ -17620,7 +17620,7 @@
       </c>
       <c r="E441" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F441" t="inlineStr">
@@ -17659,7 +17659,7 @@
       </c>
       <c r="E442" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F442" t="inlineStr">
@@ -17698,7 +17698,7 @@
       </c>
       <c r="E443" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F443" t="inlineStr">
@@ -17737,7 +17737,7 @@
       </c>
       <c r="E444" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F444" t="inlineStr">
@@ -17776,7 +17776,7 @@
       </c>
       <c r="E445" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F445" t="inlineStr">
@@ -17815,7 +17815,7 @@
       </c>
       <c r="E446" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F446" t="inlineStr">
@@ -17854,7 +17854,7 @@
       </c>
       <c r="E447" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F447" t="inlineStr">
@@ -17893,7 +17893,7 @@
       </c>
       <c r="E448" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F448" t="inlineStr">
@@ -17932,7 +17932,7 @@
       </c>
       <c r="E449" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F449" t="inlineStr">
@@ -17971,7 +17971,7 @@
       </c>
       <c r="E450" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F450" t="inlineStr">
@@ -18010,7 +18010,7 @@
       </c>
       <c r="E451" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F451" t="inlineStr">
@@ -18049,7 +18049,7 @@
       </c>
       <c r="E452" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F452" t="inlineStr">
@@ -18088,7 +18088,7 @@
       </c>
       <c r="E453" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F453" t="inlineStr">
@@ -18127,7 +18127,7 @@
       </c>
       <c r="E454" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F454" t="inlineStr">
@@ -18166,7 +18166,7 @@
       </c>
       <c r="E455" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F455" t="inlineStr">
@@ -18205,7 +18205,7 @@
       </c>
       <c r="E456" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F456" t="inlineStr">
@@ -18244,7 +18244,7 @@
       </c>
       <c r="E457" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F457" t="inlineStr">
@@ -18283,7 +18283,7 @@
       </c>
       <c r="E458" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F458" t="inlineStr">
@@ -18322,7 +18322,7 @@
       </c>
       <c r="E459" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F459" t="inlineStr">
@@ -18361,7 +18361,7 @@
       </c>
       <c r="E460" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F460" t="inlineStr">
@@ -18400,7 +18400,7 @@
       </c>
       <c r="E461" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F461" t="inlineStr">
@@ -18439,7 +18439,7 @@
       </c>
       <c r="E462" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F462" t="inlineStr">
@@ -18478,7 +18478,7 @@
       </c>
       <c r="E463" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F463" t="inlineStr">
@@ -18517,7 +18517,7 @@
       </c>
       <c r="E464" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F464" t="inlineStr">
@@ -18556,7 +18556,7 @@
       </c>
       <c r="E465" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F465" t="inlineStr">
@@ -18595,7 +18595,7 @@
       </c>
       <c r="E466" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F466" t="inlineStr">
@@ -18634,7 +18634,7 @@
       </c>
       <c r="E467" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F467" t="inlineStr">
@@ -18673,7 +18673,7 @@
       </c>
       <c r="E468" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F468" t="inlineStr">
@@ -18712,7 +18712,7 @@
       </c>
       <c r="E469" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F469" t="inlineStr">
@@ -18751,7 +18751,7 @@
       </c>
       <c r="E470" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F470" t="inlineStr">
@@ -18790,7 +18790,7 @@
       </c>
       <c r="E471" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F471" t="inlineStr">
@@ -18829,7 +18829,7 @@
       </c>
       <c r="E472" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F472" t="inlineStr">
@@ -18868,7 +18868,7 @@
       </c>
       <c r="E473" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F473" t="inlineStr">
@@ -18907,7 +18907,7 @@
       </c>
       <c r="E474" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F474" t="inlineStr">
@@ -18946,7 +18946,7 @@
       </c>
       <c r="E475" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F475" t="inlineStr">
@@ -18985,7 +18985,7 @@
       </c>
       <c r="E476" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F476" t="inlineStr">
@@ -19024,7 +19024,7 @@
       </c>
       <c r="E477" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F477" t="inlineStr">
@@ -19063,7 +19063,7 @@
       </c>
       <c r="E478" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F478" t="inlineStr">
@@ -19102,7 +19102,7 @@
       </c>
       <c r="E479" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F479" t="inlineStr">
@@ -19141,7 +19141,7 @@
       </c>
       <c r="E480" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F480" t="inlineStr">
@@ -19180,7 +19180,7 @@
       </c>
       <c r="E481" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F481" t="inlineStr">
@@ -19219,7 +19219,7 @@
       </c>
       <c r="E482" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F482" t="inlineStr">
@@ -19258,7 +19258,7 @@
       </c>
       <c r="E483" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F483" t="inlineStr">
@@ -19297,7 +19297,7 @@
       </c>
       <c r="E484" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F484" t="inlineStr">
@@ -19336,7 +19336,7 @@
       </c>
       <c r="E485" t="inlineStr">
         <is>
-          <t>1,0</t>
+          <t>1,00000</t>
         </is>
       </c>
       <c r="F485" t="inlineStr">
@@ -19375,7 +19375,7 @@
       </c>
       <c r="E486" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F486" t="inlineStr">
@@ -19414,7 +19414,7 @@
       </c>
       <c r="E487" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F487" t="inlineStr">
@@ -19453,7 +19453,7 @@
       </c>
       <c r="E488" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F488" t="inlineStr">
@@ -19492,7 +19492,7 @@
       </c>
       <c r="E489" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F489" t="inlineStr">
@@ -19531,7 +19531,7 @@
       </c>
       <c r="E490" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F490" t="inlineStr">
@@ -19570,7 +19570,7 @@
       </c>
       <c r="E491" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F491" t="inlineStr">
@@ -19609,7 +19609,7 @@
       </c>
       <c r="E492" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F492" t="inlineStr">
@@ -19648,7 +19648,7 @@
       </c>
       <c r="E493" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F493" t="inlineStr">
@@ -19687,7 +19687,7 @@
       </c>
       <c r="E494" t="inlineStr">
         <is>
-          <t>2,0</t>
+          <t>2,00000</t>
         </is>
       </c>
       <c r="F494" t="inlineStr">

</xml_diff>